<commit_message>
Added retrofit annual limit and NCAP_COST
Added a limit of 2GW per year for the retrofit plants, otherwise we retrofit too fast.
Changed the cost from a FOM to a investment cost that results in an effective additional annual payment that would raise the plant costs to the EPRI numberg
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_Power_EAF_retrofit.xlsx
+++ b/SubRes_TMPL/SubRES_Power_EAF_retrofit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA7B7C2-5D79-45DB-9954-E11F085F4646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6142B066-7612-4BDE-9429-A69EE81B3F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{D553689B-429B-4275-8EDF-B1E530A1AB9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{D553689B-429B-4275-8EDF-B1E530A1AB9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Define names" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,84 @@
     <sheet name="MTSAO_EAF_CONVERTER" sheetId="6" r:id="rId4"/>
     <sheet name="DATA" sheetId="7" r:id="rId5"/>
     <sheet name="AF and PKCNT" sheetId="8" r:id="rId6"/>
+    <sheet name="FOM calc" sheetId="9" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_AutomaticResultsDisplayMode" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceConfidenceLevel" hidden="1">0.95</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePercentileToTest" hidden="1">0.9</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformMeanTest" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformPercentileTest" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformStdDeviationTest" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTestAllOutputs" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTestingPeriod" hidden="1">100</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTolerance" hidden="1">0.03</definedName>
+    <definedName name="_AtRisk_SimSetting_LiveUpdate" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_LiveUpdatePeriod" hidden="1">-1</definedName>
+    <definedName name="_AtRisk_SimSetting_RandomNumberGenerator" hidden="1">7</definedName>
+    <definedName name="_AtRisk_SimSetting_ReportsList" hidden="1">1832</definedName>
+    <definedName name="_AtRisk_SimSetting_SimNameCount" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_SmartSensitivityAnalysisEnabled" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_StatisticFunctionUpdating" hidden="1">1</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcBehavior" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
+    <definedName name="Pal_Workbook_GUID" hidden="1">"15EKZRKTEJMR3UQGNDW1WF6V"</definedName>
+    <definedName name="RiskAfterRecalcMacro" hidden="1">""</definedName>
+    <definedName name="RiskAfterSimMacro" hidden="1">""</definedName>
+    <definedName name="RiskBeforeRecalcMacro" hidden="1">""</definedName>
+    <definedName name="RiskBeforeSimMacro" hidden="1">""</definedName>
+    <definedName name="RiskCollectDistributionSamples" hidden="1">2</definedName>
+    <definedName name="RiskFixedSeed" hidden="1">1</definedName>
+    <definedName name="RiskHasSettings" hidden="1">5</definedName>
+    <definedName name="RiskMinimizeOnStart" hidden="1">FALSE</definedName>
+    <definedName name="RiskMonitorConvergence" hidden="1">FALSE</definedName>
+    <definedName name="RiskMultipleCPUSupportEnabled" hidden="1">TRUE</definedName>
+    <definedName name="RiskNumIterations" hidden="1">5000</definedName>
+    <definedName name="RiskNumSimulations" hidden="1">1</definedName>
+    <definedName name="RiskPauseOnError" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunAfterRecalcMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunAfterSimMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunBeforeRecalcMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunBeforeSimMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskSamplingType" hidden="1">3</definedName>
+    <definedName name="RiskStandardRecalc" hidden="1">1</definedName>
+    <definedName name="RiskUpdateDisplay" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseMultipleCPUs" hidden="1">TRUE</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'FOM calc'!#REF!</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'FOM calc'!$H$36</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="254">
   <si>
     <t>Flow Efficiency</t>
   </si>
@@ -777,6 +854,54 @@
   </si>
   <si>
     <t>this is from ProcDataRM in ELC</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>R/kW</t>
+  </si>
+  <si>
+    <t>Annualized Costs</t>
+  </si>
+  <si>
+    <t>Low FOM value for the power plant</t>
+  </si>
+  <si>
+    <t>High FOM value for the power plant with retrofit</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Effective capital cost R/kW</t>
+  </si>
+  <si>
+    <t>years left</t>
+  </si>
+  <si>
+    <t>Gives annual R/kW</t>
+  </si>
+  <si>
+    <t>Unit #</t>
+  </si>
+  <si>
+    <t>Decomm schedule from ELC</t>
+  </si>
+  <si>
+    <t>Years left as of 2022</t>
+  </si>
+  <si>
+    <t>using this for the investment</t>
+  </si>
+  <si>
+    <t>R/kW/year</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1150,8 +1275,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1260,17 +1391,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1401,7 +1521,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1534,31 +1654,42 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="18" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="18" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="13" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="12" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="36" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="34" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="19" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="19" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="80">
     <cellStyle name="20% - Accent5 2" xfId="43" xr:uid="{EFF8B84A-AE81-4833-8C88-5277AC64F684}"/>
@@ -2218,6 +2349,24 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Define REFIT"/>
+      <sheetName val="Define RCAP_BND"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3127,7 +3276,7 @@
   <dimension ref="A3:AT82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8777,8 +8926,8 @@
   </sheetPr>
   <dimension ref="A3:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8788,8 +8937,7 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="16" max="17" width="13" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8816,7 +8964,7 @@
       <c r="O5" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="P5" s="88" t="s">
+      <c r="P5" s="87" t="s">
         <v>226</v>
       </c>
       <c r="Q5" s="26" t="s">
@@ -8854,10 +9002,10 @@
       <c r="N6">
         <v>2030</v>
       </c>
-      <c r="O6" s="81">
+      <c r="O6" s="80">
         <v>2034</v>
       </c>
-      <c r="P6" s="81">
+      <c r="P6" s="80">
         <v>2020</v>
       </c>
       <c r="Q6" t="s">
@@ -8871,7 +9019,7 @@
       <c r="E7" s="72"/>
       <c r="G7" s="72"/>
       <c r="O7" s="72"/>
-      <c r="P7" s="81"/>
+      <c r="P7" s="80"/>
     </row>
     <row r="8" spans="1:17" ht="34.5" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
@@ -8922,10 +9070,10 @@
         <f>"NCAP_AFA~LO~"&amp;O6</f>
         <v>NCAP_AFA~LO~2034</v>
       </c>
-      <c r="P8" s="82" t="s">
+      <c r="P8" s="81" t="s">
         <v>228</v>
       </c>
-      <c r="Q8" s="86" t="s">
+      <c r="Q8" s="85" t="s">
         <v>234</v>
       </c>
     </row>
@@ -8940,12 +9088,13 @@
       <c r="D9">
         <v>2024</v>
       </c>
-      <c r="E9" s="74">
-        <v>1</v>
-      </c>
-      <c r="F9" s="85">
-        <f>DATA!C4</f>
-        <v>841.21272918520924</v>
+      <c r="E9" s="84">
+        <f>'FOM calc'!E11</f>
+        <v>1985</v>
+      </c>
+      <c r="F9" s="84">
+        <f>MTSAO_EAF_CONVERTER!H9</f>
+        <v>543.03708177844862</v>
       </c>
       <c r="G9">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A9,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -8975,14 +9124,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A9,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
-      <c r="N9" s="80">
+      <c r="N9" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A9,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
       <c r="O9">
         <v>0.05</v>
       </c>
-      <c r="P9" s="81">
+      <c r="P9" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A9,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.67</v>
       </c>
@@ -9004,11 +9153,12 @@
         <v>2024</v>
       </c>
       <c r="E10" s="74">
-        <v>1</v>
-      </c>
-      <c r="F10" s="87">
+        <f>E9</f>
+        <v>1985</v>
+      </c>
+      <c r="F10" s="86">
         <f>F9</f>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G10">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A10,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9038,14 +9188,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A10,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
-      <c r="N10" s="80">
+      <c r="N10" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A10,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
       <c r="O10">
         <v>0.05</v>
       </c>
-      <c r="P10" s="81">
+      <c r="P10" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A10,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.6</v>
       </c>
@@ -9063,15 +9213,16 @@
         <v>ETCLEKOMA-E-REAF</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D22" si="2">D10</f>
+        <f t="shared" ref="D11:E22" si="2">D10</f>
         <v>2024</v>
       </c>
       <c r="E11" s="74">
-        <v>1</v>
-      </c>
-      <c r="F11" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F11" s="86">
         <f t="shared" ref="F11:F22" si="3">F10</f>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G11">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A11,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9101,14 +9252,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A11,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
-      <c r="N11" s="80">
+      <c r="N11" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A11,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
       <c r="O11">
         <v>0.05</v>
       </c>
-      <c r="P11" s="81">
+      <c r="P11" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A11,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.6</v>
       </c>
@@ -9130,11 +9281,12 @@
         <v>2024</v>
       </c>
       <c r="E12" s="74">
-        <v>1</v>
-      </c>
-      <c r="F12" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F12" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G12">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A12,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9164,14 +9316,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A12,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.43632000000000004</v>
       </c>
-      <c r="N12" s="80">
+      <c r="N12" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A12,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.40934999999999999</v>
       </c>
       <c r="O12">
         <v>0.05</v>
       </c>
-      <c r="P12" s="81">
+      <c r="P12" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A12,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9193,11 +9345,12 @@
         <v>2024</v>
       </c>
       <c r="E13" s="74">
-        <v>1</v>
-      </c>
-      <c r="F13" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F13" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G13">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A13,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9227,14 +9380,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A13,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.48727999999999999</v>
       </c>
-      <c r="N13" s="80">
+      <c r="N13" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A13,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.45157499999999995</v>
       </c>
       <c r="O13">
         <v>0.05</v>
       </c>
-      <c r="P13" s="81">
+      <c r="P13" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A13,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9256,11 +9409,12 @@
         <v>2024</v>
       </c>
       <c r="E14" s="74">
-        <v>1</v>
-      </c>
-      <c r="F14" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F14" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G14">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A14,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9290,14 +9444,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A14,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
-      <c r="N14" s="80">
+      <c r="N14" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A14,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0</v>
       </c>
       <c r="O14">
         <v>0.05</v>
       </c>
-      <c r="P14" s="81">
+      <c r="P14" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A14,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9319,11 +9473,12 @@
         <v>2024</v>
       </c>
       <c r="E15" s="74">
-        <v>1</v>
-      </c>
-      <c r="F15" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F15" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G15">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A15,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9353,14 +9508,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A15,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.66276000000000002</v>
       </c>
-      <c r="N15" s="80">
+      <c r="N15" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A15,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.63822499999999993</v>
       </c>
       <c r="O15">
         <v>0.05</v>
       </c>
-      <c r="P15" s="81">
+      <c r="P15" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A15,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>1</v>
       </c>
@@ -9382,11 +9537,12 @@
         <v>2024</v>
       </c>
       <c r="E16" s="74">
-        <v>1</v>
-      </c>
-      <c r="F16" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F16" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G16">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A16,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9416,14 +9572,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A16,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.48431999999999997</v>
       </c>
-      <c r="N16" s="80">
+      <c r="N16" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A16,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.48112500000000002</v>
       </c>
       <c r="O16">
         <v>0.05</v>
       </c>
-      <c r="P16" s="81">
+      <c r="P16" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A16,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9445,11 +9601,12 @@
         <v>2024</v>
       </c>
       <c r="E17" s="74">
-        <v>1</v>
-      </c>
-      <c r="F17" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F17" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G17">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A17,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9479,14 +9636,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A17,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.59248000000000001</v>
       </c>
-      <c r="N17" s="80">
+      <c r="N17" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A17,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.55020000000000002</v>
       </c>
       <c r="O17">
         <v>0.05</v>
       </c>
-      <c r="P17" s="81">
+      <c r="P17" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A17,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9508,11 +9665,12 @@
         <v>2024</v>
       </c>
       <c r="E18" s="74">
-        <v>1</v>
-      </c>
-      <c r="F18" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F18" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G18">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A18,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9542,14 +9700,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A18,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.64466999999999997</v>
       </c>
-      <c r="N18" s="80">
+      <c r="N18" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A18,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.62063750000000006</v>
       </c>
       <c r="O18">
         <v>0.05</v>
       </c>
-      <c r="P18" s="81">
+      <c r="P18" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A18,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9571,11 +9729,12 @@
         <v>2024</v>
       </c>
       <c r="E19" s="74">
-        <v>1</v>
-      </c>
-      <c r="F19" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F19" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G19">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A19,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9605,14 +9764,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A19,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.64466999999999997</v>
       </c>
-      <c r="N19" s="80">
+      <c r="N19" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A19,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.62063750000000006</v>
       </c>
       <c r="O19">
         <v>0.05</v>
       </c>
-      <c r="P19" s="81">
+      <c r="P19" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A19,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
@@ -9634,11 +9793,12 @@
         <v>2024</v>
       </c>
       <c r="E20" s="74">
-        <v>1</v>
-      </c>
-      <c r="F20" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F20" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G20">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A20,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9668,14 +9828,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A20,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.72099000000000002</v>
       </c>
-      <c r="N20" s="80">
+      <c r="N20" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A20,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.69483749999999989</v>
       </c>
       <c r="O20">
         <v>0.05</v>
       </c>
-      <c r="P20" s="81">
+      <c r="P20" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A20,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>1</v>
       </c>
@@ -9697,11 +9857,12 @@
         <v>2024</v>
       </c>
       <c r="E21" s="74">
-        <v>1</v>
-      </c>
-      <c r="F21" s="87">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F21" s="86">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G21">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A21,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9731,14 +9892,14 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A21,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.63333000000000006</v>
       </c>
-      <c r="N21" s="80">
+      <c r="N21" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A21,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.6096125</v>
       </c>
       <c r="O21">
         <v>0.05</v>
       </c>
-      <c r="P21" s="81">
+      <c r="P21" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A21,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>1</v>
       </c>
@@ -9760,12 +9921,13 @@
         <f t="shared" si="2"/>
         <v>2024</v>
       </c>
-      <c r="E22" s="76">
-        <v>1</v>
-      </c>
-      <c r="F22" s="83">
+      <c r="E22" s="74">
+        <f t="shared" si="2"/>
+        <v>1985</v>
+      </c>
+      <c r="F22" s="82">
         <f t="shared" si="3"/>
-        <v>841.21272918520924</v>
+        <v>543.03708177844862</v>
       </c>
       <c r="G22">
         <f>INDEX(MTSAO_EAF_CONVERTER!U$9:U$24,MATCH($A22,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
@@ -9795,18 +9957,18 @@
         <f>INDEX(MTSAO_EAF_CONVERTER!AA$9:AA$24,MATCH($A22,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.47023999999999999</v>
       </c>
-      <c r="N22" s="80">
+      <c r="N22" s="79">
         <f>INDEX(MTSAO_EAF_CONVERTER!AB$9:AB$24,MATCH($A22,MTSAO_EAF_CONVERTER!$D$9:$D$24,0))</f>
         <v>0.43522500000000003</v>
       </c>
-      <c r="O22" s="90">
+      <c r="O22" s="89">
         <v>0.05</v>
       </c>
-      <c r="P22" s="81">
+      <c r="P22" s="80">
         <f>INDEX('AF and PKCNT'!N$8:N$32,MATCH('Refurbishment details'!$A22,'AF and PKCNT'!$A$8:$A$21,0))</f>
         <v>0.8</v>
       </c>
-      <c r="Q22" s="84">
+      <c r="Q22" s="83">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -9820,8 +9982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB17D442-C4D0-473E-9671-D5BC1B818BD7}">
   <dimension ref="A2:AB60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11742,31 +11904,31 @@
       <c r="S31" t="s">
         <v>144</v>
       </c>
-      <c r="T31" s="91" t="s">
+      <c r="T31" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="U31" s="92">
+      <c r="U31" s="91">
         <v>0.34871200000000008</v>
       </c>
-      <c r="V31" s="92">
+      <c r="V31" s="91">
         <v>0.38320199999999999</v>
       </c>
-      <c r="W31" s="92">
+      <c r="W31" s="91">
         <v>0.51729200000000009</v>
       </c>
-      <c r="X31" s="92">
+      <c r="X31" s="91">
         <v>0.5341490000000001</v>
       </c>
-      <c r="Y31" s="92">
+      <c r="Y31" s="91">
         <v>0.53936000000000006</v>
       </c>
-      <c r="Z31" s="92">
+      <c r="Z31" s="91">
         <v>0.4864</v>
       </c>
-      <c r="AA31" s="92">
+      <c r="AA31" s="91">
         <v>0.43632000000000004</v>
       </c>
-      <c r="AB31" s="92">
+      <c r="AB31" s="91">
         <v>0.40934999999999999</v>
       </c>
     </row>
@@ -11774,31 +11936,31 @@
       <c r="S32" t="s">
         <v>144</v>
       </c>
-      <c r="T32" s="91" t="s">
+      <c r="T32" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="U32" s="92">
+      <c r="U32" s="91">
         <v>0.31875200000000004</v>
       </c>
-      <c r="V32" s="92">
+      <c r="V32" s="91">
         <v>0.38320199999999999</v>
       </c>
-      <c r="W32" s="92">
+      <c r="W32" s="91">
         <v>0.482848</v>
       </c>
-      <c r="X32" s="92">
+      <c r="X32" s="91">
         <v>0.517594</v>
       </c>
-      <c r="Y32" s="92">
+      <c r="Y32" s="91">
         <v>0.50919999999999999</v>
       </c>
-      <c r="Z32" s="92">
+      <c r="Z32" s="91">
         <v>0.47551999999999994</v>
       </c>
-      <c r="AA32" s="92">
+      <c r="AA32" s="91">
         <v>0.48727999999999999</v>
       </c>
-      <c r="AB32" s="92">
+      <c r="AB32" s="91">
         <v>0.45157499999999995</v>
       </c>
     </row>
@@ -11806,31 +11968,31 @@
       <c r="S33" t="s">
         <v>144</v>
       </c>
-      <c r="T33" s="91" t="s">
+      <c r="T33" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="U33" s="92">
+      <c r="U33" s="91">
         <v>0.38835999999999998</v>
       </c>
-      <c r="V33" s="92">
+      <c r="V33" s="91">
         <v>0.42303499999999994</v>
       </c>
-      <c r="W33" s="92">
+      <c r="W33" s="91">
         <v>0.54786499999999994</v>
       </c>
-      <c r="X33" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA33" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB33" s="92">
+      <c r="X33" s="91">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="91">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="91">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="91">
         <v>0</v>
       </c>
     </row>
@@ -11838,31 +12000,31 @@
       <c r="S34" t="s">
         <v>144</v>
       </c>
-      <c r="T34" s="91" t="s">
+      <c r="T34" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="U34" s="92">
+      <c r="U34" s="91">
         <v>0.57072600000000007</v>
       </c>
-      <c r="V34" s="92">
+      <c r="V34" s="91">
         <v>0.5556915</v>
       </c>
-      <c r="W34" s="92">
+      <c r="W34" s="91">
         <v>0.66355300000000006</v>
       </c>
-      <c r="X34" s="92">
+      <c r="X34" s="91">
         <v>0.66693600000000008</v>
       </c>
-      <c r="Y34" s="92">
+      <c r="Y34" s="91">
         <v>0.62468999999999997</v>
       </c>
-      <c r="Z34" s="92">
+      <c r="Z34" s="91">
         <v>0.71396999999999999</v>
       </c>
-      <c r="AA34" s="92">
+      <c r="AA34" s="91">
         <v>0.66276000000000002</v>
       </c>
-      <c r="AB34" s="92">
+      <c r="AB34" s="91">
         <v>0.63822499999999993</v>
       </c>
     </row>
@@ -11870,31 +12032,31 @@
       <c r="S35" t="s">
         <v>144</v>
       </c>
-      <c r="T35" s="91" t="s">
+      <c r="T35" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="U35" s="92">
+      <c r="U35" s="91">
         <v>0.28778400000000004</v>
       </c>
-      <c r="V35" s="92">
+      <c r="V35" s="91">
         <v>0.39772000000000002</v>
       </c>
-      <c r="W35" s="92">
+      <c r="W35" s="91">
         <v>0.50907599999999997</v>
       </c>
-      <c r="X35" s="92">
+      <c r="X35" s="91">
         <v>0.50350300000000003</v>
       </c>
-      <c r="Y35" s="92">
+      <c r="Y35" s="91">
         <v>0.55111999999999994</v>
       </c>
-      <c r="Z35" s="92">
+      <c r="Z35" s="91">
         <v>0.40895999999999999</v>
       </c>
-      <c r="AA35" s="92">
+      <c r="AA35" s="91">
         <v>0.48431999999999997</v>
       </c>
-      <c r="AB35" s="92">
+      <c r="AB35" s="91">
         <v>0.48112500000000002</v>
       </c>
     </row>
@@ -11902,31 +12064,31 @@
       <c r="S36" t="s">
         <v>144</v>
       </c>
-      <c r="T36" s="91" t="s">
+      <c r="T36" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="U36" s="92">
+      <c r="U36" s="91">
         <v>0.39760000000000001</v>
       </c>
-      <c r="V36" s="92">
+      <c r="V36" s="91">
         <v>0.42950099999999997</v>
       </c>
-      <c r="W36" s="92">
+      <c r="W36" s="91">
         <v>0.59155199999999997</v>
       </c>
-      <c r="X36" s="92">
+      <c r="X36" s="91">
         <v>0.52721899999999999</v>
       </c>
-      <c r="Y36" s="92">
+      <c r="Y36" s="91">
         <v>0.54327999999999999</v>
       </c>
-      <c r="Z36" s="92">
+      <c r="Z36" s="91">
         <v>0.55055999999999994</v>
       </c>
-      <c r="AA36" s="92">
+      <c r="AA36" s="91">
         <v>0.59248000000000001</v>
       </c>
-      <c r="AB36" s="92">
+      <c r="AB36" s="91">
         <v>0.55020000000000002</v>
       </c>
     </row>
@@ -11934,31 +12096,31 @@
       <c r="S37" t="s">
         <v>144</v>
       </c>
-      <c r="T37" s="91" t="s">
+      <c r="T37" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="U37" s="92">
+      <c r="U37" s="91">
         <v>0.63273600000000008</v>
       </c>
-      <c r="V37" s="92">
+      <c r="V37" s="91">
         <v>0.65366000000000002</v>
       </c>
-      <c r="W37" s="92">
+      <c r="W37" s="91">
         <v>0.70141150000000008</v>
       </c>
-      <c r="X37" s="92">
+      <c r="X37" s="91">
         <v>0.70224750000000002</v>
       </c>
-      <c r="Y37" s="92">
+      <c r="Y37" s="91">
         <v>0.70911000000000002</v>
       </c>
-      <c r="Z37" s="92">
+      <c r="Z37" s="91">
         <v>0.68805000000000005</v>
       </c>
-      <c r="AA37" s="92">
+      <c r="AA37" s="91">
         <v>0.72099000000000002</v>
       </c>
-      <c r="AB37" s="92">
+      <c r="AB37" s="91">
         <v>0.69483749999999989</v>
       </c>
     </row>
@@ -11966,31 +12128,31 @@
       <c r="S38" t="s">
         <v>144</v>
       </c>
-      <c r="T38" s="91" t="s">
+      <c r="T38" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="U38" s="92">
+      <c r="U38" s="91">
         <v>0.56643600000000005</v>
       </c>
-      <c r="V38" s="92">
+      <c r="V38" s="91">
         <v>0.59972499999999995</v>
       </c>
-      <c r="W38" s="92">
+      <c r="W38" s="91">
         <v>0.68950800000000012</v>
       </c>
-      <c r="X38" s="92">
+      <c r="X38" s="91">
         <v>0.62065049999999999</v>
       </c>
-      <c r="Y38" s="92">
+      <c r="Y38" s="91">
         <v>0.64962000000000009</v>
       </c>
-      <c r="Z38" s="92">
+      <c r="Z38" s="91">
         <v>0.64737000000000011</v>
       </c>
-      <c r="AA38" s="92">
+      <c r="AA38" s="91">
         <v>0.64466999999999997</v>
       </c>
-      <c r="AB38" s="92">
+      <c r="AB38" s="91">
         <v>0.62063750000000006</v>
       </c>
     </row>
@@ -11998,31 +12160,31 @@
       <c r="S39" t="s">
         <v>144</v>
       </c>
-      <c r="T39" s="91" t="s">
+      <c r="T39" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="U39" s="92">
+      <c r="U39" s="91">
         <v>0.553566</v>
       </c>
-      <c r="V39" s="92">
+      <c r="V39" s="91">
         <v>0.55939449999999991</v>
       </c>
-      <c r="W39" s="92">
+      <c r="W39" s="91">
         <v>0.63124350000000007</v>
       </c>
-      <c r="X39" s="92">
+      <c r="X39" s="91">
         <v>0.61649100000000001</v>
       </c>
-      <c r="Y39" s="92">
+      <c r="Y39" s="91">
         <v>0.62190000000000001</v>
       </c>
-      <c r="Z39" s="92">
+      <c r="Z39" s="91">
         <v>0.68363999999999991</v>
       </c>
-      <c r="AA39" s="92">
+      <c r="AA39" s="91">
         <v>0.63333000000000006</v>
       </c>
-      <c r="AB39" s="92">
+      <c r="AB39" s="91">
         <v>0.6096125</v>
       </c>
     </row>
@@ -12030,31 +12192,31 @@
       <c r="S40" t="s">
         <v>144</v>
       </c>
-      <c r="T40" s="91" t="s">
+      <c r="T40" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="U40" s="92">
+      <c r="U40" s="91">
         <v>0.65192400000000006</v>
       </c>
-      <c r="V40" s="92">
+      <c r="V40" s="91">
         <v>0.68585999999999991</v>
       </c>
-      <c r="W40" s="92">
+      <c r="W40" s="91">
         <v>0.73300500000000002</v>
       </c>
-      <c r="X40" s="92">
+      <c r="X40" s="91">
         <v>0.76101149999999995</v>
       </c>
-      <c r="Y40" s="92">
+      <c r="Y40" s="91">
         <v>0.77993999999999997</v>
       </c>
-      <c r="Z40" s="92">
+      <c r="Z40" s="91">
         <v>0.71567999999999998</v>
       </c>
-      <c r="AA40" s="92">
+      <c r="AA40" s="91">
         <v>0.73584000000000016</v>
       </c>
-      <c r="AB40" s="92">
+      <c r="AB40" s="91">
         <v>0.70927499999999999</v>
       </c>
     </row>
@@ -12062,31 +12224,31 @@
       <c r="S41" t="s">
         <v>144</v>
       </c>
-      <c r="T41" s="91" t="s">
+      <c r="T41" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="U41" s="92">
+      <c r="U41" s="91">
         <v>0.33124000000000003</v>
       </c>
-      <c r="V41" s="92">
+      <c r="V41" s="91">
         <v>0.33501200000000003</v>
       </c>
-      <c r="W41" s="92">
+      <c r="W41" s="91">
         <v>0.48308499999999999</v>
       </c>
-      <c r="X41" s="92">
+      <c r="X41" s="91">
         <v>0.44536800000000004</v>
       </c>
-      <c r="Y41" s="92">
+      <c r="Y41" s="91">
         <v>0.45896000000000003</v>
       </c>
-      <c r="Z41" s="92">
+      <c r="Z41" s="91">
         <v>0.50039999999999996</v>
       </c>
-      <c r="AA41" s="92">
+      <c r="AA41" s="91">
         <v>0.47023999999999999</v>
       </c>
-      <c r="AB41" s="92">
+      <c r="AB41" s="91">
         <v>0.43522500000000003</v>
       </c>
     </row>
@@ -12094,31 +12256,31 @@
       <c r="S42" t="s">
         <v>144</v>
       </c>
-      <c r="T42" s="91" t="s">
+      <c r="T42" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="U42" s="92">
+      <c r="U42" s="91">
         <v>0.63523200000000002</v>
       </c>
-      <c r="V42" s="92">
+      <c r="V42" s="91">
         <v>0.65704099999999999</v>
       </c>
-      <c r="W42" s="92">
+      <c r="W42" s="91">
         <v>0.744282</v>
       </c>
-      <c r="X42" s="92">
+      <c r="X42" s="91">
         <v>0.6921584999999999</v>
       </c>
-      <c r="Y42" s="92">
+      <c r="Y42" s="91">
         <v>0.74168999999999996</v>
       </c>
-      <c r="Z42" s="92">
+      <c r="Z42" s="91">
         <v>0.73502999999999996</v>
       </c>
-      <c r="AA42" s="92">
+      <c r="AA42" s="91">
         <v>0.72108000000000005</v>
       </c>
-      <c r="AB42" s="92">
+      <c r="AB42" s="91">
         <v>0.69492500000000001</v>
       </c>
     </row>
@@ -12126,31 +12288,31 @@
       <c r="S43" t="s">
         <v>144</v>
       </c>
-      <c r="T43" s="91" t="s">
+      <c r="T43" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="U43" s="92">
+      <c r="U43" s="91">
         <v>0.36215200000000008</v>
       </c>
-      <c r="V43" s="92">
+      <c r="V43" s="91">
         <v>0.38466600000000001</v>
       </c>
-      <c r="W43" s="92">
+      <c r="W43" s="91">
         <v>0.49817400000000006</v>
       </c>
-      <c r="X43" s="92">
+      <c r="X43" s="91">
         <v>0.48556200000000005</v>
       </c>
-      <c r="Y43" s="92">
+      <c r="Y43" s="91">
         <v>0.50448000000000004</v>
       </c>
-      <c r="Z43" s="92">
+      <c r="Z43" s="91">
         <v>0.50448000000000004</v>
       </c>
-      <c r="AA43" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB43" s="92">
+      <c r="AA43" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="91">
         <v>0</v>
       </c>
     </row>
@@ -12158,31 +12320,31 @@
       <c r="S44" t="s">
         <v>144</v>
       </c>
-      <c r="T44" s="91" t="s">
+      <c r="T44" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="U44" s="92">
-        <v>0</v>
-      </c>
-      <c r="V44" s="92">
-        <v>0</v>
-      </c>
-      <c r="W44" s="92">
-        <v>0</v>
-      </c>
-      <c r="X44" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA44" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="92">
+      <c r="U44" s="91">
+        <v>0</v>
+      </c>
+      <c r="V44" s="91">
+        <v>0</v>
+      </c>
+      <c r="W44" s="91">
+        <v>0</v>
+      </c>
+      <c r="X44" s="91">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="91">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="91">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="91">
         <v>0</v>
       </c>
     </row>
@@ -12190,31 +12352,31 @@
       <c r="S45" t="s">
         <v>144</v>
       </c>
-      <c r="T45" s="91" t="s">
+      <c r="T45" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="U45" s="92">
-        <v>0</v>
-      </c>
-      <c r="V45" s="92">
-        <v>0</v>
-      </c>
-      <c r="W45" s="92">
-        <v>0</v>
-      </c>
-      <c r="X45" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA45" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="92">
+      <c r="U45" s="91">
+        <v>0</v>
+      </c>
+      <c r="V45" s="91">
+        <v>0</v>
+      </c>
+      <c r="W45" s="91">
+        <v>0</v>
+      </c>
+      <c r="X45" s="91">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="91">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="91">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="91">
         <v>0</v>
       </c>
     </row>
@@ -12222,31 +12384,31 @@
       <c r="S46" t="s">
         <v>135</v>
       </c>
-      <c r="T46" s="91" t="s">
+      <c r="T46" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="U46" s="92">
+      <c r="U46" s="91">
         <v>0.34871200000000008</v>
       </c>
-      <c r="V46" s="92">
+      <c r="V46" s="91">
         <v>0.28269</v>
       </c>
-      <c r="W46" s="92">
+      <c r="W46" s="91">
         <v>0.25537200000000004</v>
       </c>
-      <c r="X46" s="92">
+      <c r="X46" s="91">
         <v>0.22892100000000004</v>
       </c>
-      <c r="Y46" s="92">
+      <c r="Y46" s="91">
         <v>0.23596999999999999</v>
       </c>
-      <c r="Z46" s="92">
+      <c r="Z46" s="91">
         <v>0.20064000000000001</v>
       </c>
-      <c r="AA46" s="92">
+      <c r="AA46" s="91">
         <v>0.17452799999999999</v>
       </c>
-      <c r="AB46" s="92">
+      <c r="AB46" s="91">
         <v>0.13644999999999999</v>
       </c>
     </row>
@@ -12254,31 +12416,31 @@
       <c r="S47" t="s">
         <v>135</v>
       </c>
-      <c r="T47" s="91" t="s">
+      <c r="T47" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="U47" s="92">
+      <c r="U47" s="91">
         <v>0.31875200000000004</v>
       </c>
-      <c r="V47" s="92">
+      <c r="V47" s="91">
         <v>0.28269</v>
       </c>
-      <c r="W47" s="92">
+      <c r="W47" s="91">
         <v>0.238368</v>
       </c>
-      <c r="X47" s="92">
+      <c r="X47" s="91">
         <v>0.22182600000000002</v>
       </c>
-      <c r="Y47" s="92">
+      <c r="Y47" s="91">
         <v>0.22277499999999997</v>
       </c>
-      <c r="Z47" s="92">
+      <c r="Z47" s="91">
         <v>0.19615199999999999</v>
       </c>
-      <c r="AA47" s="92">
+      <c r="AA47" s="91">
         <v>0.194912</v>
       </c>
-      <c r="AB47" s="92">
+      <c r="AB47" s="91">
         <v>0.15052499999999999</v>
       </c>
     </row>
@@ -12286,31 +12448,31 @@
       <c r="S48" t="s">
         <v>135</v>
       </c>
-      <c r="T48" s="91" t="s">
+      <c r="T48" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="U48" s="92">
+      <c r="U48" s="91">
         <v>0.38835999999999998</v>
       </c>
-      <c r="V48" s="92">
+      <c r="V48" s="91">
         <v>0.31207499999999994</v>
       </c>
-      <c r="W48" s="92">
+      <c r="W48" s="91">
         <v>0.27046499999999996</v>
       </c>
-      <c r="X48" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z48" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA48" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB48" s="92">
+      <c r="X48" s="91">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="91">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="91">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="91">
         <v>0</v>
       </c>
     </row>
@@ -12318,31 +12480,31 @@
       <c r="S49" t="s">
         <v>135</v>
       </c>
-      <c r="T49" s="91" t="s">
+      <c r="T49" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="U49" s="92">
+      <c r="U49" s="91">
         <v>0.57072600000000007</v>
       </c>
-      <c r="V49" s="92">
+      <c r="V49" s="91">
         <v>0.50046749999999995</v>
       </c>
-      <c r="W49" s="92">
+      <c r="W49" s="91">
         <v>0.51527300000000009</v>
       </c>
-      <c r="X49" s="92">
+      <c r="X49" s="91">
         <v>0.50114400000000003</v>
       </c>
-      <c r="Y49" s="92">
+      <c r="Y49" s="91">
         <v>0.46851749999999998</v>
       </c>
-      <c r="Z49" s="92">
+      <c r="Z49" s="91">
         <v>0.52754450000000008</v>
       </c>
-      <c r="AA49" s="92">
+      <c r="AA49" s="91">
         <v>0.48602400000000007</v>
       </c>
-      <c r="AB49" s="92">
+      <c r="AB49" s="91">
         <v>0.45587499999999997</v>
       </c>
     </row>
@@ -12350,31 +12512,31 @@
       <c r="S50" t="s">
         <v>135</v>
       </c>
-      <c r="T50" s="91" t="s">
+      <c r="T50" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="U50" s="92">
+      <c r="U50" s="91">
         <v>0.28778400000000004</v>
       </c>
-      <c r="V50" s="92">
+      <c r="V50" s="91">
         <v>0.29339999999999999</v>
       </c>
-      <c r="W50" s="92">
+      <c r="W50" s="91">
         <v>0.25131599999999998</v>
       </c>
-      <c r="X50" s="92">
+      <c r="X50" s="91">
         <v>0.21578700000000003</v>
       </c>
-      <c r="Y50" s="92">
+      <c r="Y50" s="91">
         <v>0.24111499999999997</v>
       </c>
-      <c r="Z50" s="92">
+      <c r="Z50" s="91">
         <v>0.16869600000000001</v>
       </c>
-      <c r="AA50" s="92">
+      <c r="AA50" s="91">
         <v>0.19372799999999998</v>
       </c>
-      <c r="AB50" s="92">
+      <c r="AB50" s="91">
         <v>0.16037500000000002</v>
       </c>
     </row>
@@ -12382,31 +12544,31 @@
       <c r="S51" t="s">
         <v>135</v>
       </c>
-      <c r="T51" s="91" t="s">
+      <c r="T51" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="U51" s="92">
+      <c r="U51" s="91">
         <v>0.39760000000000001</v>
       </c>
-      <c r="V51" s="92">
+      <c r="V51" s="91">
         <v>0.31684499999999999</v>
       </c>
-      <c r="W51" s="92">
+      <c r="W51" s="91">
         <v>0.29203199999999996</v>
       </c>
-      <c r="X51" s="92">
+      <c r="X51" s="91">
         <v>0.22595100000000001</v>
       </c>
-      <c r="Y51" s="92">
+      <c r="Y51" s="91">
         <v>0.23768499999999995</v>
       </c>
-      <c r="Z51" s="92">
+      <c r="Z51" s="91">
         <v>0.22710599999999997</v>
       </c>
-      <c r="AA51" s="92">
+      <c r="AA51" s="91">
         <v>0.23699200000000001</v>
       </c>
-      <c r="AB51" s="92">
+      <c r="AB51" s="91">
         <v>0.18340000000000001</v>
       </c>
     </row>
@@ -12414,31 +12576,31 @@
       <c r="S52" t="s">
         <v>135</v>
       </c>
-      <c r="T52" s="91" t="s">
+      <c r="T52" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="U52" s="92">
+      <c r="U52" s="91">
         <v>0.63273600000000008</v>
       </c>
-      <c r="V52" s="92">
+      <c r="V52" s="91">
         <v>0.5887</v>
       </c>
-      <c r="W52" s="92">
+      <c r="W52" s="91">
         <v>0.54467150000000009</v>
       </c>
-      <c r="X52" s="92">
+      <c r="X52" s="91">
         <v>0.52767750000000002</v>
       </c>
-      <c r="Y52" s="92">
+      <c r="Y52" s="91">
         <v>0.53183250000000004</v>
       </c>
-      <c r="Z52" s="92">
+      <c r="Z52" s="91">
         <v>0.50839250000000002</v>
       </c>
-      <c r="AA52" s="92">
+      <c r="AA52" s="91">
         <v>0.52872600000000003</v>
       </c>
-      <c r="AB52" s="92">
+      <c r="AB52" s="91">
         <v>0.49631249999999993</v>
       </c>
     </row>
@@ -12446,31 +12608,31 @@
       <c r="S53" t="s">
         <v>135</v>
       </c>
-      <c r="T53" s="91" t="s">
+      <c r="T53" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="U53" s="92">
+      <c r="U53" s="91">
         <v>0.56643600000000005</v>
       </c>
-      <c r="V53" s="92">
+      <c r="V53" s="91">
         <v>0.54012499999999997</v>
       </c>
-      <c r="W53" s="92">
+      <c r="W53" s="91">
         <v>0.53542800000000013</v>
       </c>
-      <c r="X53" s="92">
+      <c r="X53" s="91">
         <v>0.46636449999999996</v>
       </c>
-      <c r="Y53" s="92">
+      <c r="Y53" s="91">
         <v>0.48721500000000012</v>
       </c>
-      <c r="Z53" s="92">
+      <c r="Z53" s="91">
         <v>0.47833450000000005</v>
       </c>
-      <c r="AA53" s="92">
+      <c r="AA53" s="91">
         <v>0.47275799999999996</v>
       </c>
-      <c r="AB53" s="92">
+      <c r="AB53" s="91">
         <v>0.4433125</v>
       </c>
     </row>
@@ -12478,31 +12640,31 @@
       <c r="S54" t="s">
         <v>135</v>
       </c>
-      <c r="T54" s="91" t="s">
+      <c r="T54" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="U54" s="92">
+      <c r="U54" s="91">
         <v>0.553566</v>
       </c>
-      <c r="V54" s="92">
+      <c r="V54" s="91">
         <v>0.50380249999999993</v>
       </c>
-      <c r="W54" s="92">
+      <c r="W54" s="91">
         <v>0.49018350000000005</v>
       </c>
-      <c r="X54" s="92">
+      <c r="X54" s="91">
         <v>0.46323900000000001</v>
       </c>
-      <c r="Y54" s="92">
+      <c r="Y54" s="91">
         <v>0.46642499999999998</v>
       </c>
-      <c r="Z54" s="92">
+      <c r="Z54" s="91">
         <v>0.50513399999999997</v>
       </c>
-      <c r="AA54" s="92">
+      <c r="AA54" s="91">
         <v>0.46444200000000002</v>
       </c>
-      <c r="AB54" s="92">
+      <c r="AB54" s="91">
         <v>0.43543749999999998</v>
       </c>
     </row>
@@ -12510,31 +12672,31 @@
       <c r="S55" t="s">
         <v>135</v>
       </c>
-      <c r="T55" s="91" t="s">
+      <c r="T55" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="U55" s="92">
+      <c r="U55" s="91">
         <v>0.65192400000000006</v>
       </c>
-      <c r="V55" s="92">
+      <c r="V55" s="91">
         <v>0.61769999999999992</v>
       </c>
-      <c r="W55" s="92">
+      <c r="W55" s="91">
         <v>0.56920500000000007</v>
       </c>
-      <c r="X55" s="92">
+      <c r="X55" s="91">
         <v>0.57183349999999999</v>
       </c>
-      <c r="Y55" s="92">
+      <c r="Y55" s="91">
         <v>0.584955</v>
       </c>
-      <c r="Z55" s="92">
+      <c r="Z55" s="91">
         <v>0.52880799999999994</v>
       </c>
-      <c r="AA55" s="92">
+      <c r="AA55" s="91">
         <v>0.5396160000000001</v>
       </c>
-      <c r="AB55" s="92">
+      <c r="AB55" s="91">
         <v>0.50662499999999999</v>
       </c>
     </row>
@@ -12542,31 +12704,31 @@
       <c r="S56" t="s">
         <v>135</v>
       </c>
-      <c r="T56" s="91" t="s">
+      <c r="T56" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="U56" s="92">
+      <c r="U56" s="91">
         <v>0.33124000000000003</v>
       </c>
-      <c r="V56" s="92">
+      <c r="V56" s="91">
         <v>0.24714000000000003</v>
       </c>
-      <c r="W56" s="92">
+      <c r="W56" s="91">
         <v>0.23848499999999997</v>
       </c>
-      <c r="X56" s="92">
+      <c r="X56" s="91">
         <v>0.19087200000000001</v>
       </c>
-      <c r="Y56" s="92">
+      <c r="Y56" s="91">
         <v>0.20079499999999997</v>
       </c>
-      <c r="Z56" s="92">
+      <c r="Z56" s="91">
         <v>0.20641499999999999</v>
       </c>
-      <c r="AA56" s="92">
+      <c r="AA56" s="91">
         <v>0.18809600000000001</v>
       </c>
-      <c r="AB56" s="92">
+      <c r="AB56" s="91">
         <v>0.14507500000000001</v>
       </c>
     </row>
@@ -12574,31 +12736,31 @@
       <c r="S57" t="s">
         <v>135</v>
       </c>
-      <c r="T57" s="91" t="s">
+      <c r="T57" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="U57" s="92">
+      <c r="U57" s="91">
         <v>0.63523200000000002</v>
       </c>
-      <c r="V57" s="92">
+      <c r="V57" s="91">
         <v>0.59174499999999997</v>
       </c>
-      <c r="W57" s="92">
+      <c r="W57" s="91">
         <v>0.57796200000000009</v>
       </c>
-      <c r="X57" s="92">
+      <c r="X57" s="91">
         <v>0.52009649999999996</v>
       </c>
-      <c r="Y57" s="92">
+      <c r="Y57" s="91">
         <v>0.55626750000000003</v>
       </c>
-      <c r="Z57" s="92">
+      <c r="Z57" s="91">
         <v>0.54310550000000002</v>
       </c>
-      <c r="AA57" s="92">
+      <c r="AA57" s="91">
         <v>0.52879200000000004</v>
       </c>
-      <c r="AB57" s="92">
+      <c r="AB57" s="91">
         <v>0.49637500000000001</v>
       </c>
     </row>
@@ -12606,31 +12768,31 @@
       <c r="S58" t="s">
         <v>135</v>
       </c>
-      <c r="T58" s="91" t="s">
+      <c r="T58" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="U58" s="92">
+      <c r="U58" s="91">
         <v>0.36215200000000008</v>
       </c>
-      <c r="V58" s="92">
+      <c r="V58" s="91">
         <v>0.28377000000000002</v>
       </c>
-      <c r="W58" s="92">
+      <c r="W58" s="91">
         <v>0.24593400000000004</v>
       </c>
-      <c r="X58" s="92">
+      <c r="X58" s="91">
         <v>0.20809800000000003</v>
       </c>
-      <c r="Y58" s="92">
+      <c r="Y58" s="91">
         <v>0.22070999999999999</v>
       </c>
-      <c r="Z58" s="92">
+      <c r="Z58" s="91">
         <v>0.20809800000000003</v>
       </c>
-      <c r="AA58" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB58" s="92">
+      <c r="AA58" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="91">
         <v>0</v>
       </c>
     </row>
@@ -12638,31 +12800,31 @@
       <c r="S59" t="s">
         <v>135</v>
       </c>
-      <c r="T59" s="91" t="s">
+      <c r="T59" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="U59" s="92">
-        <v>0</v>
-      </c>
-      <c r="V59" s="92">
-        <v>0</v>
-      </c>
-      <c r="W59" s="92">
-        <v>0</v>
-      </c>
-      <c r="X59" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA59" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB59" s="92">
+      <c r="U59" s="91">
+        <v>0</v>
+      </c>
+      <c r="V59" s="91">
+        <v>0</v>
+      </c>
+      <c r="W59" s="91">
+        <v>0</v>
+      </c>
+      <c r="X59" s="91">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="91">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="91">
+        <v>0</v>
+      </c>
+      <c r="AA59" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB59" s="91">
         <v>0</v>
       </c>
     </row>
@@ -12670,31 +12832,31 @@
       <c r="S60" t="s">
         <v>135</v>
       </c>
-      <c r="T60" s="91" t="s">
+      <c r="T60" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="U60" s="92">
-        <v>0</v>
-      </c>
-      <c r="V60" s="92">
-        <v>0</v>
-      </c>
-      <c r="W60" s="92">
-        <v>0</v>
-      </c>
-      <c r="X60" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA60" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="92">
+      <c r="U60" s="91">
+        <v>0</v>
+      </c>
+      <c r="V60" s="91">
+        <v>0</v>
+      </c>
+      <c r="W60" s="91">
+        <v>0</v>
+      </c>
+      <c r="X60" s="91">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="91">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="91">
+        <v>0</v>
+      </c>
+      <c r="AA60" s="91">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="91">
         <v>0</v>
       </c>
     </row>
@@ -14519,13 +14681,13 @@
       <c r="N6" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="O6" s="79" t="s">
+      <c r="O6" s="78" t="s">
         <v>229</v>
       </c>
-      <c r="P6" s="79" t="s">
+      <c r="P6" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="Q6" s="79" t="s">
+      <c r="Q6" s="78" t="s">
         <v>231</v>
       </c>
       <c r="R6" s="3" t="str">
@@ -14564,7 +14726,7 @@
       <c r="V7" s="2"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="88" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -14628,7 +14790,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="88" t="s">
         <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -14692,7 +14854,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="88" t="s">
         <v>97</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -14756,7 +14918,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="88" t="s">
         <v>94</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -14820,7 +14982,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="88" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -14884,7 +15046,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="88" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -14948,7 +15110,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="88" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -15012,7 +15174,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="88" t="s">
         <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -15076,7 +15238,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="88" t="s">
         <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -15140,7 +15302,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="88" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -15204,7 +15366,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="88" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -15268,7 +15430,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="88" t="s">
         <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -15332,7 +15494,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="89" t="s">
+      <c r="A20" s="88" t="s">
         <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -15396,7 +15558,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="88" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -15464,7 +15626,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="77"/>
+      <c r="G22" s="76"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -15519,11 +15681,11 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
       <c r="M25" s="8"/>
       <c r="N25" s="15"/>
       <c r="R25" s="15"/>
@@ -15591,11 +15753,11 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
+      <c r="L29" s="77"/>
       <c r="M29" s="8"/>
       <c r="N29" s="15"/>
       <c r="R29" s="15"/>
@@ -15675,4 +15837,2047 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6465C81B-59B8-49B1-9788-631F5AE7974E}">
+  <dimension ref="A1:AI55"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="92"/>
+    <col min="3" max="3" width="15.140625" style="92" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="92"/>
+    <col min="5" max="5" width="9.5703125" style="92" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="92" customWidth="1"/>
+    <col min="7" max="12" width="9.140625" style="92"/>
+    <col min="13" max="13" width="10.42578125" style="92" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="92"/>
+    <col min="15" max="15" width="23" style="92" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="92"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C1" s="92" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="92" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="99">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J1" s="92" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="J2" s="33">
+        <v>543.03708177844862</v>
+      </c>
+      <c r="K2" s="92" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="J3" s="32">
+        <v>841.21272918520924</v>
+      </c>
+      <c r="K3" s="92" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C4" s="96" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" s="92" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" s="94"/>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="J5" s="95">
+        <f>J3-J2</f>
+        <v>298.17564740676062</v>
+      </c>
+      <c r="K5" s="92" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="92" t="s">
+        <v>245</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="92" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="92" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C7" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="97"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="93"/>
+    </row>
+    <row r="8" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C8" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="97"/>
+      <c r="F8" s="95"/>
+    </row>
+    <row r="9" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C9" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="97"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="93"/>
+    </row>
+    <row r="10" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C10" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="97"/>
+      <c r="F10" s="95"/>
+    </row>
+    <row r="11" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C11" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="101">
+        <f>A34</f>
+        <v>10</v>
+      </c>
+      <c r="E11" s="102">
+        <v>1985</v>
+      </c>
+      <c r="F11" s="103">
+        <f>-PMT($E$1,$D11,$E11)</f>
+        <v>298.49763792475858</v>
+      </c>
+      <c r="H11" s="92" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C12" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="97"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+    </row>
+    <row r="13" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C13" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="97"/>
+      <c r="F13" s="95"/>
+    </row>
+    <row r="14" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C14" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="95"/>
+    </row>
+    <row r="15" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C15" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="95"/>
+    </row>
+    <row r="16" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="C16" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="95"/>
+    </row>
+    <row r="17" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="C17" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="95"/>
+    </row>
+    <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="C18" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="95"/>
+    </row>
+    <row r="19" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="C19" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="95"/>
+    </row>
+    <row r="20" spans="1:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="C20" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="95"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="D22" s="93"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="97"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="G23" s="97"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="D24" s="93"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="D25" s="93"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="C26" s="92" t="s">
+        <v>250</v>
+      </c>
+      <c r="D26" s="93"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="D27" s="93"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" s="92" t="s">
+        <v>251</v>
+      </c>
+      <c r="D28" s="93"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="C29" s="92" t="s">
+        <v>249</v>
+      </c>
+      <c r="D29" s="96">
+        <v>2019</v>
+      </c>
+      <c r="E29" s="98">
+        <v>2020</v>
+      </c>
+      <c r="F29" s="98">
+        <v>2021</v>
+      </c>
+      <c r="G29" s="98">
+        <v>2022</v>
+      </c>
+      <c r="H29" s="96">
+        <v>2023</v>
+      </c>
+      <c r="I29" s="96">
+        <v>2024</v>
+      </c>
+      <c r="J29" s="96">
+        <v>2025</v>
+      </c>
+      <c r="K29" s="96">
+        <v>2026</v>
+      </c>
+      <c r="L29" s="96">
+        <v>2027</v>
+      </c>
+      <c r="M29" s="96">
+        <v>2028</v>
+      </c>
+      <c r="N29" s="96">
+        <v>2029</v>
+      </c>
+      <c r="O29" s="96">
+        <v>2030</v>
+      </c>
+      <c r="P29" s="96">
+        <v>2031</v>
+      </c>
+      <c r="Q29" s="96">
+        <v>2032</v>
+      </c>
+      <c r="R29" s="96">
+        <v>2033</v>
+      </c>
+      <c r="S29" s="96">
+        <v>2034</v>
+      </c>
+      <c r="T29" s="96">
+        <v>2035</v>
+      </c>
+      <c r="U29" s="96">
+        <v>2036</v>
+      </c>
+      <c r="V29" s="96">
+        <v>2037</v>
+      </c>
+      <c r="W29" s="96">
+        <v>2038</v>
+      </c>
+      <c r="X29" s="96">
+        <v>2039</v>
+      </c>
+      <c r="Y29" s="96">
+        <v>2040</v>
+      </c>
+      <c r="Z29" s="96">
+        <v>2041</v>
+      </c>
+      <c r="AA29" s="96">
+        <v>2042</v>
+      </c>
+      <c r="AB29" s="96">
+        <v>2043</v>
+      </c>
+      <c r="AC29" s="96">
+        <v>2044</v>
+      </c>
+      <c r="AD29" s="96">
+        <v>2045</v>
+      </c>
+      <c r="AE29" s="96">
+        <v>2046</v>
+      </c>
+      <c r="AF29" s="96">
+        <v>2047</v>
+      </c>
+      <c r="AG29" s="96">
+        <v>2048</v>
+      </c>
+      <c r="AH29" s="96">
+        <v>2049</v>
+      </c>
+      <c r="AI29" s="96">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A30" s="92">
+        <f>COUNT($I$29:$AI$29)-COUNTIF(I30:AI30,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C30" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="92">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="E30" s="97">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="F30" s="97">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="G30" s="97">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="H30" s="92">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="I30" s="92">
+        <v>1.0578571428571428</v>
+      </c>
+      <c r="J30" s="92">
+        <v>0.63471428571428568</v>
+      </c>
+      <c r="K30" s="92">
+        <v>0</v>
+      </c>
+      <c r="L30" s="92">
+        <v>0</v>
+      </c>
+      <c r="M30" s="92">
+        <v>0</v>
+      </c>
+      <c r="N30" s="92">
+        <v>0</v>
+      </c>
+      <c r="O30" s="92">
+        <v>0</v>
+      </c>
+      <c r="P30" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="92">
+        <v>0</v>
+      </c>
+      <c r="R30" s="92">
+        <v>0</v>
+      </c>
+      <c r="S30" s="92">
+        <v>0</v>
+      </c>
+      <c r="T30" s="92">
+        <v>0</v>
+      </c>
+      <c r="U30" s="92">
+        <v>0</v>
+      </c>
+      <c r="V30" s="92">
+        <v>0</v>
+      </c>
+      <c r="W30" s="92">
+        <v>0</v>
+      </c>
+      <c r="X30" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A31" s="92">
+        <f t="shared" ref="A31:A45" si="0">COUNT($I$29:$AI$29)-COUNTIF(I31:AI31,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C31" s="92" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="92">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E31" s="97">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F31" s="97">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G31" s="97">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H31" s="92">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I31" s="92">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J31" s="92">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K31" s="92">
+        <v>0.38</v>
+      </c>
+      <c r="L31" s="92">
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="M31" s="92">
+        <v>0</v>
+      </c>
+      <c r="N31" s="92">
+        <v>0</v>
+      </c>
+      <c r="O31" s="92">
+        <v>0</v>
+      </c>
+      <c r="P31" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="92">
+        <v>0</v>
+      </c>
+      <c r="R31" s="92">
+        <v>0</v>
+      </c>
+      <c r="S31" s="92">
+        <v>0</v>
+      </c>
+      <c r="T31" s="92">
+        <v>0</v>
+      </c>
+      <c r="U31" s="92">
+        <v>0</v>
+      </c>
+      <c r="V31" s="92">
+        <v>0</v>
+      </c>
+      <c r="W31" s="92">
+        <v>0</v>
+      </c>
+      <c r="X31" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A32" s="92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C32" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="92">
+        <v>0.41</v>
+      </c>
+      <c r="E32" s="95">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F32" s="95">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="G32" s="92">
+        <v>0</v>
+      </c>
+      <c r="H32" s="92">
+        <v>0</v>
+      </c>
+      <c r="I32" s="92">
+        <v>0</v>
+      </c>
+      <c r="J32" s="92">
+        <v>0</v>
+      </c>
+      <c r="K32" s="92">
+        <v>0</v>
+      </c>
+      <c r="L32" s="92">
+        <v>0</v>
+      </c>
+      <c r="M32" s="92">
+        <v>0</v>
+      </c>
+      <c r="N32" s="92">
+        <v>0</v>
+      </c>
+      <c r="O32" s="92">
+        <v>0</v>
+      </c>
+      <c r="P32" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="92">
+        <v>0</v>
+      </c>
+      <c r="R32" s="92">
+        <v>0</v>
+      </c>
+      <c r="S32" s="92">
+        <v>0</v>
+      </c>
+      <c r="T32" s="92">
+        <v>0</v>
+      </c>
+      <c r="U32" s="92">
+        <v>0</v>
+      </c>
+      <c r="V32" s="92">
+        <v>0</v>
+      </c>
+      <c r="W32" s="92">
+        <v>0</v>
+      </c>
+      <c r="X32" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A33" s="92">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C33" s="92" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="92">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="E33" s="95">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="F33" s="95">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="G33" s="92">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="H33" s="92">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="I33" s="92">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="J33" s="92">
+        <v>2.2320000000000002</v>
+      </c>
+      <c r="K33" s="92">
+        <v>1.488</v>
+      </c>
+      <c r="L33" s="92">
+        <v>0.74399999999999988</v>
+      </c>
+      <c r="M33" s="92">
+        <v>0.74399999999999988</v>
+      </c>
+      <c r="N33" s="92">
+        <v>0</v>
+      </c>
+      <c r="O33" s="92">
+        <v>0</v>
+      </c>
+      <c r="P33" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="92">
+        <v>0</v>
+      </c>
+      <c r="R33" s="92">
+        <v>0</v>
+      </c>
+      <c r="S33" s="92">
+        <v>0</v>
+      </c>
+      <c r="T33" s="92">
+        <v>0</v>
+      </c>
+      <c r="U33" s="92">
+        <v>0</v>
+      </c>
+      <c r="V33" s="92">
+        <v>0</v>
+      </c>
+      <c r="W33" s="92">
+        <v>0</v>
+      </c>
+      <c r="X33" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A34" s="92">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C34" s="92" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="E34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="F34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="G34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="H34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="I34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="J34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="K34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="L34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="M34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="N34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="O34" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="P34" s="92">
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="Q34" s="92">
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="R34" s="92">
+        <v>0.57500000000000018</v>
+      </c>
+      <c r="S34" s="92">
+        <v>0</v>
+      </c>
+      <c r="T34" s="92">
+        <v>0</v>
+      </c>
+      <c r="U34" s="92">
+        <v>0</v>
+      </c>
+      <c r="V34" s="92">
+        <v>0</v>
+      </c>
+      <c r="W34" s="92">
+        <v>0</v>
+      </c>
+      <c r="X34" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A35" s="92">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C35" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="92">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="E35" s="92">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="F35" s="92">
+        <v>1.1082857142857143</v>
+      </c>
+      <c r="G35" s="92">
+        <v>1.1082857142857143</v>
+      </c>
+      <c r="H35" s="92">
+        <v>0.9235714285714286</v>
+      </c>
+      <c r="I35" s="92">
+        <v>0.73885714285714288</v>
+      </c>
+      <c r="J35" s="92">
+        <v>0</v>
+      </c>
+      <c r="K35" s="92">
+        <v>0</v>
+      </c>
+      <c r="L35" s="92">
+        <v>0</v>
+      </c>
+      <c r="M35" s="92">
+        <v>0</v>
+      </c>
+      <c r="N35" s="92">
+        <v>0</v>
+      </c>
+      <c r="O35" s="92">
+        <v>0</v>
+      </c>
+      <c r="P35" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="92">
+        <v>0</v>
+      </c>
+      <c r="R35" s="92">
+        <v>0</v>
+      </c>
+      <c r="S35" s="92">
+        <v>0</v>
+      </c>
+      <c r="T35" s="92">
+        <v>0</v>
+      </c>
+      <c r="U35" s="92">
+        <v>0</v>
+      </c>
+      <c r="V35" s="92">
+        <v>0</v>
+      </c>
+      <c r="W35" s="92">
+        <v>0</v>
+      </c>
+      <c r="X35" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A36" s="92">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C36" s="92" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="E36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="F36" s="97">
+        <v>3.84</v>
+      </c>
+      <c r="G36" s="97">
+        <v>3.84</v>
+      </c>
+      <c r="H36" s="97">
+        <v>3.84</v>
+      </c>
+      <c r="I36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="J36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="K36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="L36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="M36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="N36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="O36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="P36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="Q36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="R36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="S36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="T36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="U36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="V36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="W36" s="92">
+        <v>3.84</v>
+      </c>
+      <c r="X36" s="92">
+        <v>3.1999999999999997</v>
+      </c>
+      <c r="Y36" s="92">
+        <v>3.1999999999999997</v>
+      </c>
+      <c r="Z36" s="92">
+        <v>2.5599999999999996</v>
+      </c>
+      <c r="AA36" s="92">
+        <v>1.2799999999999996</v>
+      </c>
+      <c r="AB36" s="92">
+        <v>0.63999999999999957</v>
+      </c>
+      <c r="AC36" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A37" s="92">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C37" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="92">
+        <v>2.85</v>
+      </c>
+      <c r="E37" s="92">
+        <v>2.85</v>
+      </c>
+      <c r="F37" s="97">
+        <v>2.85</v>
+      </c>
+      <c r="G37" s="97">
+        <v>2.85</v>
+      </c>
+      <c r="H37" s="92">
+        <v>2.85</v>
+      </c>
+      <c r="I37" s="92">
+        <v>2.85</v>
+      </c>
+      <c r="J37" s="92">
+        <v>2.85</v>
+      </c>
+      <c r="K37" s="92">
+        <v>2.375</v>
+      </c>
+      <c r="L37" s="92">
+        <v>1.9</v>
+      </c>
+      <c r="M37" s="92">
+        <v>1.4249999999999998</v>
+      </c>
+      <c r="N37" s="92">
+        <v>0.47499999999999976</v>
+      </c>
+      <c r="O37" s="92">
+        <v>0</v>
+      </c>
+      <c r="P37" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="92">
+        <v>0</v>
+      </c>
+      <c r="R37" s="92">
+        <v>0</v>
+      </c>
+      <c r="S37" s="92">
+        <v>0</v>
+      </c>
+      <c r="T37" s="92">
+        <v>0</v>
+      </c>
+      <c r="U37" s="92">
+        <v>0</v>
+      </c>
+      <c r="V37" s="92">
+        <v>0</v>
+      </c>
+      <c r="W37" s="92">
+        <v>0</v>
+      </c>
+      <c r="X37" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A38" s="92">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C38" s="92" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="E38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="F38" s="97">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="G38" s="97">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="H38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="I38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="J38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="K38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="L38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="M38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="N38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="O38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="P38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="Q38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="R38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="S38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="T38" s="92">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="U38" s="92">
+        <v>2.9649999999999999</v>
+      </c>
+      <c r="V38" s="92">
+        <v>1.7789999999999999</v>
+      </c>
+      <c r="W38" s="92">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="X38" s="92">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="Y38" s="92">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="Z38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A39" s="92">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C39" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="E39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="F39" s="97">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="G39" s="97">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="H39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="I39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="J39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="K39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="L39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="M39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="N39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="O39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="P39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="Q39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="R39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="S39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="T39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="U39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="V39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="W39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="X39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="Y39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="Z39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="AA39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="AB39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="AC39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="AD39" s="92">
+        <v>1.8330000000000002</v>
+      </c>
+      <c r="AE39" s="92">
+        <v>1.222</v>
+      </c>
+      <c r="AF39" s="92">
+        <v>0.61099999999999988</v>
+      </c>
+      <c r="AG39" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A40" s="92">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F40" s="97">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G40" s="97">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="H40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="I40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="J40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="K40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="L40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="M40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="N40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="O40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="P40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Q40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="R40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="S40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="T40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="U40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="V40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="W40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="X40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Y40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Z40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AA40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AB40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AC40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AD40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AE40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AF40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AG40" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AH40" s="92">
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="AI40" s="92">
+        <v>0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A41" s="92">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C41" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="E41" s="95">
+        <v>3.69</v>
+      </c>
+      <c r="F41" s="97">
+        <v>3.69</v>
+      </c>
+      <c r="G41" s="97">
+        <v>3.69</v>
+      </c>
+      <c r="H41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="I41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="J41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="K41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="L41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="M41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="N41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="O41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="P41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="Q41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="R41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="S41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="T41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="U41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="V41" s="92">
+        <v>3.69</v>
+      </c>
+      <c r="W41" s="92">
+        <v>2.46</v>
+      </c>
+      <c r="X41" s="92">
+        <v>1.845</v>
+      </c>
+      <c r="Y41" s="92">
+        <v>1.23</v>
+      </c>
+      <c r="Z41" s="92">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="AA41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI41" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A42" s="92">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C42" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="E42" s="95">
+        <v>3.45</v>
+      </c>
+      <c r="F42" s="97">
+        <v>3.45</v>
+      </c>
+      <c r="G42" s="97">
+        <v>3.45</v>
+      </c>
+      <c r="H42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="I42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="J42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="K42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="L42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="M42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="N42" s="92">
+        <v>3.45</v>
+      </c>
+      <c r="O42" s="92">
+        <v>2.875</v>
+      </c>
+      <c r="P42" s="92">
+        <v>1.7249999999999999</v>
+      </c>
+      <c r="Q42" s="92">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R42" s="92">
+        <v>0.57499999999999984</v>
+      </c>
+      <c r="S42" s="92">
+        <v>0</v>
+      </c>
+      <c r="T42" s="92">
+        <v>0</v>
+      </c>
+      <c r="U42" s="92">
+        <v>0</v>
+      </c>
+      <c r="V42" s="92">
+        <v>0</v>
+      </c>
+      <c r="W42" s="92">
+        <v>0</v>
+      </c>
+      <c r="X42" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A43" s="92">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C43" s="92" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="E43" s="95">
+        <v>3.51</v>
+      </c>
+      <c r="F43" s="97">
+        <v>3.51</v>
+      </c>
+      <c r="G43" s="97">
+        <v>3.51</v>
+      </c>
+      <c r="H43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="I43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="J43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="K43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="L43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="M43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="N43" s="92">
+        <v>3.51</v>
+      </c>
+      <c r="O43" s="92">
+        <v>0</v>
+      </c>
+      <c r="P43" s="92">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="92">
+        <v>0</v>
+      </c>
+      <c r="R43" s="92">
+        <v>0</v>
+      </c>
+      <c r="S43" s="92">
+        <v>0</v>
+      </c>
+      <c r="T43" s="92">
+        <v>0</v>
+      </c>
+      <c r="U43" s="92">
+        <v>0</v>
+      </c>
+      <c r="V43" s="92">
+        <v>0</v>
+      </c>
+      <c r="W43" s="92">
+        <v>0</v>
+      </c>
+      <c r="X43" s="92">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="92">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="92">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A44" s="92">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C44" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="92">
+        <v>33.601999999999997</v>
+      </c>
+      <c r="E44" s="95">
+        <v>33.396999999999998</v>
+      </c>
+      <c r="F44" s="97">
+        <v>33.109785714285707</v>
+      </c>
+      <c r="G44" s="97">
+        <v>33.007285714285707</v>
+      </c>
+      <c r="H44" s="92">
+        <v>32.822571428571422</v>
+      </c>
+      <c r="I44" s="92">
+        <v>32.21471428571428</v>
+      </c>
+      <c r="J44" s="92">
+        <v>31.052714285714281</v>
+      </c>
+      <c r="K44" s="92">
+        <v>29.009</v>
+      </c>
+      <c r="L44" s="92">
+        <v>27.6</v>
+      </c>
+      <c r="M44" s="92">
+        <v>26.935000000000002</v>
+      </c>
+      <c r="N44" s="92">
+        <v>25.241</v>
+      </c>
+      <c r="O44" s="92">
+        <v>20.681000000000001</v>
+      </c>
+      <c r="P44" s="92">
+        <v>18.381</v>
+      </c>
+      <c r="Q44" s="92">
+        <v>17.805999999999997</v>
+      </c>
+      <c r="R44" s="92">
+        <v>16.081</v>
+      </c>
+      <c r="S44" s="92">
+        <v>14.930999999999999</v>
+      </c>
+      <c r="T44" s="92">
+        <v>14.930999999999999</v>
+      </c>
+      <c r="U44" s="92">
+        <v>14.337999999999999</v>
+      </c>
+      <c r="V44" s="92">
+        <v>13.151999999999999</v>
+      </c>
+      <c r="W44" s="92">
+        <v>11.329000000000001</v>
+      </c>
+      <c r="X44" s="92">
+        <v>10.074</v>
+      </c>
+      <c r="Y44" s="92">
+        <v>8.8659999999999997</v>
+      </c>
+      <c r="Z44" s="92">
+        <v>7.0179999999999998</v>
+      </c>
+      <c r="AA44" s="92">
+        <v>5.1229999999999993</v>
+      </c>
+      <c r="AB44" s="92">
+        <v>4.4829999999999997</v>
+      </c>
+      <c r="AC44" s="92">
+        <v>3.843</v>
+      </c>
+      <c r="AD44" s="92">
+        <v>3.843</v>
+      </c>
+      <c r="AE44" s="92">
+        <v>3.2319999999999998</v>
+      </c>
+      <c r="AF44" s="92">
+        <v>2.6209999999999996</v>
+      </c>
+      <c r="AG44" s="92">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AH44" s="92">
+        <v>1.3399999999999999</v>
+      </c>
+      <c r="AI44" s="92">
+        <v>0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A45" s="92">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C45" s="92" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="92">
+        <v>-0.20499999999999829</v>
+      </c>
+      <c r="F45" s="92">
+        <v>-0.28721428571429186</v>
+      </c>
+      <c r="G45" s="92">
+        <v>-0.10249999999999915</v>
+      </c>
+      <c r="H45" s="92">
+        <v>-0.18471428571428561</v>
+      </c>
+      <c r="I45" s="92">
+        <v>-0.60785714285714221</v>
+      </c>
+      <c r="J45" s="92">
+        <v>-1.161999999999999</v>
+      </c>
+      <c r="K45" s="92">
+        <v>-2.0437142857142803</v>
+      </c>
+      <c r="L45" s="92">
+        <v>-1.4089999999999989</v>
+      </c>
+      <c r="M45" s="92">
+        <v>-0.66499999999999915</v>
+      </c>
+      <c r="N45" s="92">
+        <v>-1.6940000000000026</v>
+      </c>
+      <c r="O45" s="92">
+        <v>-4.5599999999999987</v>
+      </c>
+      <c r="P45" s="92">
+        <v>-2.3000000000000007</v>
+      </c>
+      <c r="Q45" s="92">
+        <v>-0.57500000000000284</v>
+      </c>
+      <c r="R45" s="92">
+        <v>-1.7249999999999979</v>
+      </c>
+      <c r="S45" s="92">
+        <v>-1.1500000000000004</v>
+      </c>
+      <c r="T45" s="92">
+        <v>0</v>
+      </c>
+      <c r="U45" s="92">
+        <v>-0.59299999999999997</v>
+      </c>
+      <c r="V45" s="92">
+        <v>-1.1859999999999999</v>
+      </c>
+      <c r="W45" s="92">
+        <v>-1.8229999999999986</v>
+      </c>
+      <c r="X45" s="92">
+        <v>-1.2550000000000008</v>
+      </c>
+      <c r="Y45" s="92">
+        <v>-1.2080000000000002</v>
+      </c>
+      <c r="Z45" s="92">
+        <v>-1.8479999999999999</v>
+      </c>
+      <c r="AA45" s="92">
+        <v>-1.8950000000000005</v>
+      </c>
+      <c r="AB45" s="92">
+        <v>-0.63999999999999968</v>
+      </c>
+      <c r="AC45" s="92">
+        <v>-0.63999999999999968</v>
+      </c>
+      <c r="AD45" s="92">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="92">
+        <v>-0.61100000000000021</v>
+      </c>
+      <c r="AF45" s="92">
+        <v>-0.61100000000000021</v>
+      </c>
+      <c r="AG45" s="92">
+        <v>-0.61099999999999977</v>
+      </c>
+      <c r="AH45" s="92">
+        <v>-0.66999999999999993</v>
+      </c>
+      <c r="AI45" s="92">
+        <v>-0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="C46" s="96"/>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="D48" s="93"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="93"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="93"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="93"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="93"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="93"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="93"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="93"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>